<commit_message>
Korrektur der regulären Ausdrücke, um Änderung im Haupttext zu berücksichtigen. Kleinere Erweiterungen beim Logging. Zusätzliche Erläuterungen im Markdown des Abfrage-Notebooks.
</commit_message>
<xml_diff>
--- a/data/c19stats-ac-kennzahlen.xlsx
+++ b/data/c19stats-ac-kennzahlen.xlsx
@@ -440,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U161"/>
+  <dimension ref="A1:U164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10657,20 +10657,35 @@
       <c r="G159">
         <v>0</v>
       </c>
+      <c r="H159">
+        <v>4.142857142857143</v>
+      </c>
       <c r="I159">
         <v>0</v>
       </c>
+      <c r="J159">
+        <v>7.58876576486639</v>
+      </c>
       <c r="K159">
         <v>0</v>
       </c>
       <c r="L159">
         <v>0</v>
       </c>
+      <c r="M159">
+        <v>8.857142857142858</v>
+      </c>
       <c r="N159">
         <v>0</v>
       </c>
+      <c r="O159">
+        <v>0</v>
+      </c>
       <c r="P159">
         <v>0</v>
+      </c>
+      <c r="Q159">
+        <v>4.714285714285714</v>
       </c>
       <c r="R159">
         <v>385.0827684912641</v>
@@ -10707,20 +10722,35 @@
       <c r="G160">
         <v>1</v>
       </c>
+      <c r="H160">
+        <v>2.428571428571428</v>
+      </c>
       <c r="I160">
         <v>1.234567901234568</v>
       </c>
+      <c r="J160">
+        <v>5.402847679270441</v>
+      </c>
       <c r="K160">
         <v>18</v>
       </c>
       <c r="L160">
         <v>7</v>
       </c>
+      <c r="M160">
+        <v>8.857142857142858</v>
+      </c>
       <c r="N160">
+        <v>0</v>
+      </c>
+      <c r="O160">
         <v>0</v>
       </c>
       <c r="P160">
         <v>17</v>
+      </c>
+      <c r="Q160">
+        <v>6.428571428571429</v>
       </c>
       <c r="R160">
         <v>388.3232966973616</v>
@@ -10757,20 +10787,35 @@
       <c r="G161">
         <v>0</v>
       </c>
+      <c r="H161">
+        <v>2.428571428571428</v>
+      </c>
       <c r="I161">
         <v>0</v>
       </c>
+      <c r="J161">
+        <v>5.402847679270441</v>
+      </c>
       <c r="K161">
         <v>0</v>
       </c>
       <c r="L161">
         <v>0</v>
       </c>
+      <c r="M161">
+        <v>8.857142857142858</v>
+      </c>
       <c r="N161">
         <v>0</v>
       </c>
+      <c r="O161">
+        <v>0</v>
+      </c>
       <c r="P161">
         <v>0</v>
+      </c>
+      <c r="Q161">
+        <v>6.428571428571429</v>
       </c>
       <c r="R161">
         <v>388.3232966973616</v>
@@ -10782,6 +10827,156 @@
         <v>11.72285552591155</v>
       </c>
       <c r="U161">
+        <v>11.16181937655838</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21">
+      <c r="A162" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B162">
+        <v>2157</v>
+      </c>
+      <c r="C162">
+        <v>1060</v>
+      </c>
+      <c r="D162">
+        <v>100</v>
+      </c>
+      <c r="E162">
+        <v>1975</v>
+      </c>
+      <c r="F162">
+        <v>82</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+      <c r="I162">
+        <v>0</v>
+      </c>
+      <c r="K162">
+        <v>0</v>
+      </c>
+      <c r="L162">
+        <v>0</v>
+      </c>
+      <c r="N162">
+        <v>0</v>
+      </c>
+      <c r="P162">
+        <v>0</v>
+      </c>
+      <c r="R162">
+        <v>388.3232966973616</v>
+      </c>
+      <c r="S162">
+        <v>428.4905812919395</v>
+      </c>
+      <c r="T162">
+        <v>11.72285552591155</v>
+      </c>
+      <c r="U162">
+        <v>11.16181937655838</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21">
+      <c r="A163" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B163">
+        <v>2170</v>
+      </c>
+      <c r="C163">
+        <v>1068</v>
+      </c>
+      <c r="D163">
+        <v>100</v>
+      </c>
+      <c r="E163">
+        <v>1999</v>
+      </c>
+      <c r="F163">
+        <v>71</v>
+      </c>
+      <c r="G163">
+        <v>-11</v>
+      </c>
+      <c r="I163">
+        <v>-13.41463414634146</v>
+      </c>
+      <c r="K163">
+        <v>13</v>
+      </c>
+      <c r="L163">
+        <v>8</v>
+      </c>
+      <c r="N163">
+        <v>0</v>
+      </c>
+      <c r="P163">
+        <v>24</v>
+      </c>
+      <c r="R163">
+        <v>390.6636781795433</v>
+      </c>
+      <c r="S163">
+        <v>431.7244724715013</v>
+      </c>
+      <c r="T163">
+        <v>11.31861912846633</v>
+      </c>
+      <c r="U163">
+        <v>11.16181937655838</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21">
+      <c r="A164" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B164">
+        <v>2170</v>
+      </c>
+      <c r="C164">
+        <v>1068</v>
+      </c>
+      <c r="D164">
+        <v>100</v>
+      </c>
+      <c r="E164">
+        <v>1999</v>
+      </c>
+      <c r="F164">
+        <v>71</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="I164">
+        <v>0</v>
+      </c>
+      <c r="K164">
+        <v>0</v>
+      </c>
+      <c r="L164">
+        <v>0</v>
+      </c>
+      <c r="N164">
+        <v>0</v>
+      </c>
+      <c r="P164">
+        <v>0</v>
+      </c>
+      <c r="R164">
+        <v>390.6636781795433</v>
+      </c>
+      <c r="S164">
+        <v>431.7244724715013</v>
+      </c>
+      <c r="T164">
+        <v>11.31861912846633</v>
+      </c>
+      <c r="U164">
         <v>11.16181937655838</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pattern für reguläre Ausdrücke korrigiert.
</commit_message>
<xml_diff>
--- a/data/c19stats-ac-kennzahlen.xlsx
+++ b/data/c19stats-ac-kennzahlen.xlsx
@@ -440,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U164"/>
+  <dimension ref="A1:U168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10852,20 +10852,35 @@
       <c r="G162">
         <v>0</v>
       </c>
+      <c r="H162">
+        <v>-1.285714285714286</v>
+      </c>
       <c r="I162">
         <v>0</v>
       </c>
+      <c r="J162">
+        <v>-1.538802220125937</v>
+      </c>
       <c r="K162">
         <v>0</v>
       </c>
       <c r="L162">
         <v>0</v>
       </c>
+      <c r="M162">
+        <v>6</v>
+      </c>
       <c r="N162">
         <v>0</v>
       </c>
+      <c r="O162">
+        <v>0.1428571428571428</v>
+      </c>
       <c r="P162">
         <v>0</v>
+      </c>
+      <c r="Q162">
+        <v>7.142857142857143</v>
       </c>
       <c r="R162">
         <v>388.3232966973616</v>
@@ -10902,20 +10917,35 @@
       <c r="G163">
         <v>-11</v>
       </c>
+      <c r="H163">
+        <v>-1.285714285714286</v>
+      </c>
       <c r="I163">
         <v>-13.41463414634146</v>
       </c>
+      <c r="J163">
+        <v>-1.538802220125937</v>
+      </c>
       <c r="K163">
         <v>13</v>
       </c>
       <c r="L163">
         <v>8</v>
       </c>
+      <c r="M163">
+        <v>6</v>
+      </c>
       <c r="N163">
         <v>0</v>
+      </c>
+      <c r="O163">
+        <v>0.1428571428571428</v>
       </c>
       <c r="P163">
         <v>24</v>
+      </c>
+      <c r="Q163">
+        <v>7.142857142857143</v>
       </c>
       <c r="R163">
         <v>390.6636781795433</v>
@@ -10952,20 +10982,35 @@
       <c r="G164">
         <v>0</v>
       </c>
+      <c r="H164">
+        <v>0.1428571428571428</v>
+      </c>
       <c r="I164">
         <v>0</v>
       </c>
+      <c r="J164">
+        <v>0.4673706193802354</v>
+      </c>
       <c r="K164">
         <v>0</v>
       </c>
       <c r="L164">
         <v>0</v>
       </c>
+      <c r="M164">
+        <v>7.857142857142857</v>
+      </c>
       <c r="N164">
         <v>0</v>
       </c>
+      <c r="O164">
+        <v>0.1428571428571428</v>
+      </c>
       <c r="P164">
         <v>0</v>
+      </c>
+      <c r="Q164">
+        <v>7.571428571428571</v>
       </c>
       <c r="R164">
         <v>390.6636781795433</v>
@@ -10978,6 +11023,221 @@
       </c>
       <c r="U164">
         <v>11.16181937655838</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21">
+      <c r="A165" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B165">
+        <v>2181</v>
+      </c>
+      <c r="C165">
+        <v>1070</v>
+      </c>
+      <c r="D165">
+        <v>101</v>
+      </c>
+      <c r="E165">
+        <v>2008</v>
+      </c>
+      <c r="F165">
+        <v>72</v>
+      </c>
+      <c r="G165">
+        <v>1</v>
+      </c>
+      <c r="H165">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="I165">
+        <v>1.408450704225352</v>
+      </c>
+      <c r="J165">
+        <v>0.4673706193802354</v>
+      </c>
+      <c r="K165">
+        <v>11</v>
+      </c>
+      <c r="L165">
+        <v>2</v>
+      </c>
+      <c r="M165">
+        <v>7.857142857142857</v>
+      </c>
+      <c r="N165">
+        <v>1</v>
+      </c>
+      <c r="O165">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P165">
+        <v>9</v>
+      </c>
+      <c r="Q165">
+        <v>7.571428571428571</v>
+      </c>
+      <c r="R165">
+        <v>392.6440009721584</v>
+      </c>
+      <c r="S165">
+        <v>432.5329452663918</v>
+      </c>
+      <c r="T165">
+        <v>6.872018756568841</v>
+      </c>
+      <c r="U165">
+        <v>7.561232480894385</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21">
+      <c r="A166" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B166">
+        <v>2181</v>
+      </c>
+      <c r="C166">
+        <v>1070</v>
+      </c>
+      <c r="D166">
+        <v>101</v>
+      </c>
+      <c r="E166">
+        <v>2008</v>
+      </c>
+      <c r="F166">
+        <v>72</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="I166">
+        <v>0</v>
+      </c>
+      <c r="K166">
+        <v>0</v>
+      </c>
+      <c r="L166">
+        <v>0</v>
+      </c>
+      <c r="N166">
+        <v>0</v>
+      </c>
+      <c r="P166">
+        <v>0</v>
+      </c>
+      <c r="R166">
+        <v>392.6440009721584</v>
+      </c>
+      <c r="S166">
+        <v>432.5329452663918</v>
+      </c>
+      <c r="T166">
+        <v>6.872018756568841</v>
+      </c>
+      <c r="U166">
+        <v>7.561232480894385</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21">
+      <c r="A167" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B167">
+        <v>2212</v>
+      </c>
+      <c r="C167">
+        <v>1088</v>
+      </c>
+      <c r="D167">
+        <v>101</v>
+      </c>
+      <c r="E167">
+        <v>2028</v>
+      </c>
+      <c r="F167">
+        <v>83</v>
+      </c>
+      <c r="G167">
+        <v>11</v>
+      </c>
+      <c r="I167">
+        <v>15.27777777777778</v>
+      </c>
+      <c r="K167">
+        <v>31</v>
+      </c>
+      <c r="L167">
+        <v>18</v>
+      </c>
+      <c r="N167">
+        <v>0</v>
+      </c>
+      <c r="P167">
+        <v>20</v>
+      </c>
+      <c r="R167">
+        <v>398.2249106604377</v>
+      </c>
+      <c r="S167">
+        <v>439.8092004204058</v>
+      </c>
+      <c r="T167">
+        <v>11.31861912846633</v>
+      </c>
+      <c r="U167">
+        <v>9.901613963075981</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21">
+      <c r="A168" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B168">
+        <v>2212</v>
+      </c>
+      <c r="C168">
+        <v>1088</v>
+      </c>
+      <c r="D168">
+        <v>101</v>
+      </c>
+      <c r="E168">
+        <v>2028</v>
+      </c>
+      <c r="F168">
+        <v>83</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="I168">
+        <v>0</v>
+      </c>
+      <c r="K168">
+        <v>0</v>
+      </c>
+      <c r="L168">
+        <v>0</v>
+      </c>
+      <c r="N168">
+        <v>0</v>
+      </c>
+      <c r="P168">
+        <v>0</v>
+      </c>
+      <c r="R168">
+        <v>398.2249106604377</v>
+      </c>
+      <c r="S168">
+        <v>439.8092004204058</v>
+      </c>
+      <c r="T168">
+        <v>11.31861912846633</v>
+      </c>
+      <c r="U168">
+        <v>9.901613963075981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Neues Notebook für den Import manuell eingegebener Daten hinzugefügt.
</commit_message>
<xml_diff>
--- a/data/c19stats-ac-kennzahlen.xlsx
+++ b/data/c19stats-ac-kennzahlen.xlsx
@@ -440,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U171"/>
+  <dimension ref="A1:U210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -11307,20 +11307,35 @@
       <c r="G169">
         <v>0</v>
       </c>
+      <c r="H169">
+        <v>1.857142857142857</v>
+      </c>
       <c r="I169">
         <v>0</v>
       </c>
+      <c r="J169">
+        <v>2.604005766656367</v>
+      </c>
       <c r="K169">
         <v>0</v>
       </c>
       <c r="L169">
         <v>0</v>
       </c>
+      <c r="M169">
+        <v>9.571428571428571</v>
+      </c>
       <c r="N169">
         <v>0</v>
       </c>
+      <c r="O169">
+        <v>0</v>
+      </c>
       <c r="P169">
         <v>0</v>
+      </c>
+      <c r="Q169">
+        <v>7.714285714285714</v>
       </c>
       <c r="R169">
         <v>398.2249106604377</v>
@@ -11357,20 +11372,35 @@
       <c r="G170">
         <v>-5</v>
       </c>
+      <c r="H170">
+        <v>1.857142857142857</v>
+      </c>
       <c r="I170">
         <v>-6.024096385542169</v>
       </c>
+      <c r="J170">
+        <v>2.604005766656367</v>
+      </c>
       <c r="K170">
         <v>20</v>
       </c>
       <c r="L170">
         <v>5</v>
       </c>
+      <c r="M170">
+        <v>11.42857142857143</v>
+      </c>
       <c r="N170">
         <v>0</v>
+      </c>
+      <c r="O170">
+        <v>0.1428571428571428</v>
       </c>
       <c r="P170">
         <v>25</v>
+      </c>
+      <c r="Q170">
+        <v>9.428571428571429</v>
       </c>
       <c r="R170">
         <v>401.8254975561017</v>
@@ -11407,20 +11437,35 @@
       <c r="G171">
         <v>0</v>
       </c>
+      <c r="H171">
+        <v>1.714285714285714</v>
+      </c>
       <c r="I171">
         <v>0</v>
       </c>
+      <c r="J171">
+        <v>2.102138353024247</v>
+      </c>
       <c r="K171">
         <v>0</v>
       </c>
       <c r="L171">
         <v>0</v>
       </c>
+      <c r="M171">
+        <v>8.857142857142858</v>
+      </c>
       <c r="N171">
         <v>0</v>
       </c>
+      <c r="O171">
+        <v>0.1428571428571428</v>
+      </c>
       <c r="P171">
         <v>0</v>
+      </c>
+      <c r="Q171">
+        <v>7</v>
       </c>
       <c r="R171">
         <v>401.8254975561017</v>
@@ -11433,6 +11478,2496 @@
       </c>
       <c r="U171">
         <v>11.16181937655838</v>
+      </c>
+    </row>
+    <row r="172" spans="1:21">
+      <c r="A172" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B172">
+        <v>2248</v>
+      </c>
+      <c r="C172">
+        <v>1102</v>
+      </c>
+      <c r="D172">
+        <v>101</v>
+      </c>
+      <c r="E172">
+        <v>2062</v>
+      </c>
+      <c r="F172">
+        <v>85</v>
+      </c>
+      <c r="G172">
+        <v>7</v>
+      </c>
+      <c r="H172">
+        <v>1.285714285714286</v>
+      </c>
+      <c r="I172">
+        <v>8.974358974358974</v>
+      </c>
+      <c r="J172">
+        <v>1.651010533475374</v>
+      </c>
+      <c r="K172">
+        <v>16</v>
+      </c>
+      <c r="L172">
+        <v>9</v>
+      </c>
+      <c r="M172">
+        <v>9.857142857142858</v>
+      </c>
+      <c r="N172">
+        <v>0</v>
+      </c>
+      <c r="O172">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P172">
+        <v>9</v>
+      </c>
+      <c r="Q172">
+        <v>8.428571428571429</v>
+      </c>
+      <c r="R172">
+        <v>404.7059670726328</v>
+      </c>
+      <c r="S172">
+        <v>445.4685099846391</v>
+      </c>
+      <c r="T172">
+        <v>12.93556471824723</v>
+      </c>
+      <c r="U172">
+        <v>12.06196610047438</v>
+      </c>
+    </row>
+    <row r="173" spans="1:21">
+      <c r="A173" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B173">
+        <v>2261</v>
+      </c>
+      <c r="C173">
+        <v>1106</v>
+      </c>
+      <c r="D173">
+        <v>102</v>
+      </c>
+      <c r="E173">
+        <v>2074</v>
+      </c>
+      <c r="F173">
+        <v>85</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="H173">
+        <v>1.285714285714286</v>
+      </c>
+      <c r="I173">
+        <v>0</v>
+      </c>
+      <c r="J173">
+        <v>1.651010533475374</v>
+      </c>
+      <c r="K173">
+        <v>13</v>
+      </c>
+      <c r="L173">
+        <v>4</v>
+      </c>
+      <c r="M173">
+        <v>9.857142857142858</v>
+      </c>
+      <c r="N173">
+        <v>1</v>
+      </c>
+      <c r="O173">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P173">
+        <v>12</v>
+      </c>
+      <c r="Q173">
+        <v>8.428571428571429</v>
+      </c>
+      <c r="R173">
+        <v>407.0463485548144</v>
+      </c>
+      <c r="S173">
+        <v>447.0854555744199</v>
+      </c>
+      <c r="T173">
+        <v>14.55251030802813</v>
+      </c>
+      <c r="U173">
+        <v>14.40234758265597</v>
+      </c>
+    </row>
+    <row r="174" spans="1:21">
+      <c r="A174" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B174">
+        <v>2274</v>
+      </c>
+      <c r="C174">
+        <v>1112</v>
+      </c>
+      <c r="D174">
+        <v>102</v>
+      </c>
+      <c r="E174">
+        <v>2077</v>
+      </c>
+      <c r="F174">
+        <v>95</v>
+      </c>
+      <c r="G174">
+        <v>10</v>
+      </c>
+      <c r="H174">
+        <v>1.571428571428571</v>
+      </c>
+      <c r="I174">
+        <v>11.76470588235294</v>
+      </c>
+      <c r="J174">
+        <v>2.0457572220932</v>
+      </c>
+      <c r="K174">
+        <v>13</v>
+      </c>
+      <c r="L174">
+        <v>6</v>
+      </c>
+      <c r="M174">
+        <v>11.28571428571429</v>
+      </c>
+      <c r="N174">
+        <v>0</v>
+      </c>
+      <c r="O174">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P174">
+        <v>3</v>
+      </c>
+      <c r="Q174">
+        <v>9.571428571428571</v>
+      </c>
+      <c r="R174">
+        <v>409.386730036996</v>
+      </c>
+      <c r="S174">
+        <v>449.5108739590913</v>
+      </c>
+      <c r="T174">
+        <v>9.701673538685423</v>
+      </c>
+      <c r="U174">
+        <v>11.16181937655838</v>
+      </c>
+    </row>
+    <row r="175" spans="1:21">
+      <c r="A175" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B175">
+        <v>2281</v>
+      </c>
+      <c r="C175">
+        <v>1114</v>
+      </c>
+      <c r="D175">
+        <v>102</v>
+      </c>
+      <c r="E175">
+        <v>2087</v>
+      </c>
+      <c r="F175">
+        <v>92</v>
+      </c>
+      <c r="G175">
+        <v>-3</v>
+      </c>
+      <c r="H175">
+        <v>1.571428571428571</v>
+      </c>
+      <c r="I175">
+        <v>-3.157894736842105</v>
+      </c>
+      <c r="J175">
+        <v>2.0457572220932</v>
+      </c>
+      <c r="K175">
+        <v>7</v>
+      </c>
+      <c r="L175">
+        <v>2</v>
+      </c>
+      <c r="M175">
+        <v>11.28571428571429</v>
+      </c>
+      <c r="N175">
+        <v>0</v>
+      </c>
+      <c r="O175">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P175">
+        <v>10</v>
+      </c>
+      <c r="Q175">
+        <v>9.571428571428571</v>
+      </c>
+      <c r="R175">
+        <v>410.6469354504785</v>
+      </c>
+      <c r="S175">
+        <v>450.3193467539817</v>
+      </c>
+      <c r="T175">
+        <v>10.51014633357588</v>
+      </c>
+      <c r="U175">
+        <v>12.42202479004078</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21">
+      <c r="A176" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B176">
+        <v>2281</v>
+      </c>
+      <c r="C176">
+        <v>1114</v>
+      </c>
+      <c r="D176">
+        <v>102</v>
+      </c>
+      <c r="E176">
+        <v>2087</v>
+      </c>
+      <c r="F176">
+        <v>92</v>
+      </c>
+      <c r="G176">
+        <v>0</v>
+      </c>
+      <c r="H176">
+        <v>-2</v>
+      </c>
+      <c r="I176">
+        <v>0</v>
+      </c>
+      <c r="J176">
+        <v>-2.125539645832881</v>
+      </c>
+      <c r="K176">
+        <v>0</v>
+      </c>
+      <c r="L176">
+        <v>0</v>
+      </c>
+      <c r="M176">
+        <v>9.714285714285714</v>
+      </c>
+      <c r="N176">
+        <v>0</v>
+      </c>
+      <c r="O176">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P176">
+        <v>0</v>
+      </c>
+      <c r="Q176">
+        <v>11.57142857142857</v>
+      </c>
+      <c r="R176">
+        <v>410.6469354504785</v>
+      </c>
+      <c r="S176">
+        <v>450.3193467539817</v>
+      </c>
+      <c r="T176">
+        <v>10.51014633357588</v>
+      </c>
+      <c r="U176">
+        <v>12.42202479004078</v>
+      </c>
+    </row>
+    <row r="177" spans="1:21">
+      <c r="A177" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B177">
+        <v>2311</v>
+      </c>
+      <c r="C177">
+        <v>1126</v>
+      </c>
+      <c r="D177">
+        <v>102</v>
+      </c>
+      <c r="E177">
+        <v>2120</v>
+      </c>
+      <c r="F177">
+        <v>89</v>
+      </c>
+      <c r="G177">
+        <v>-3</v>
+      </c>
+      <c r="H177">
+        <v>-1.714285714285714</v>
+      </c>
+      <c r="I177">
+        <v>-3.260869565217391</v>
+      </c>
+      <c r="J177">
+        <v>-1.723125158911352</v>
+      </c>
+      <c r="K177">
+        <v>30</v>
+      </c>
+      <c r="L177">
+        <v>12</v>
+      </c>
+      <c r="M177">
+        <v>9</v>
+      </c>
+      <c r="N177">
+        <v>0</v>
+      </c>
+      <c r="O177">
+        <v>0</v>
+      </c>
+      <c r="P177">
+        <v>33</v>
+      </c>
+      <c r="Q177">
+        <v>10.71428571428571</v>
+      </c>
+      <c r="R177">
+        <v>416.0478157939744</v>
+      </c>
+      <c r="S177">
+        <v>455.1701835233245</v>
+      </c>
+      <c r="T177">
+        <v>13.33980111569246</v>
+      </c>
+      <c r="U177">
+        <v>14.22231823787277</v>
+      </c>
+    </row>
+    <row r="178" spans="1:21">
+      <c r="A178" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B178">
+        <v>2311</v>
+      </c>
+      <c r="C178">
+        <v>1126</v>
+      </c>
+      <c r="D178">
+        <v>102</v>
+      </c>
+      <c r="E178">
+        <v>2120</v>
+      </c>
+      <c r="F178">
+        <v>89</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+      <c r="H178">
+        <v>-2.857142857142857</v>
+      </c>
+      <c r="I178">
+        <v>0</v>
+      </c>
+      <c r="J178">
+        <v>-3.012407995333592</v>
+      </c>
+      <c r="K178">
+        <v>0</v>
+      </c>
+      <c r="L178">
+        <v>0</v>
+      </c>
+      <c r="M178">
+        <v>8.428571428571429</v>
+      </c>
+      <c r="N178">
+        <v>0</v>
+      </c>
+      <c r="O178">
+        <v>0</v>
+      </c>
+      <c r="P178">
+        <v>0</v>
+      </c>
+      <c r="Q178">
+        <v>11.28571428571429</v>
+      </c>
+      <c r="R178">
+        <v>416.0478157939744</v>
+      </c>
+      <c r="S178">
+        <v>455.1701835233245</v>
+      </c>
+      <c r="T178">
+        <v>13.33980111569246</v>
+      </c>
+      <c r="U178">
+        <v>14.22231823787277</v>
+      </c>
+    </row>
+    <row r="179" spans="1:21">
+      <c r="A179" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B179">
+        <v>2316</v>
+      </c>
+      <c r="C179">
+        <v>1128</v>
+      </c>
+      <c r="D179">
+        <v>102</v>
+      </c>
+      <c r="E179">
+        <v>2143</v>
+      </c>
+      <c r="F179">
+        <v>71</v>
+      </c>
+      <c r="G179">
+        <v>-18</v>
+      </c>
+      <c r="H179">
+        <v>-1.285714285714286</v>
+      </c>
+      <c r="I179">
+        <v>-20.22471910112359</v>
+      </c>
+      <c r="J179">
+        <v>-1.037470651975196</v>
+      </c>
+      <c r="K179">
+        <v>5</v>
+      </c>
+      <c r="L179">
+        <v>2</v>
+      </c>
+      <c r="M179">
+        <v>9.571428571428571</v>
+      </c>
+      <c r="N179">
+        <v>0</v>
+      </c>
+      <c r="O179">
+        <v>0</v>
+      </c>
+      <c r="P179">
+        <v>23</v>
+      </c>
+      <c r="Q179">
+        <v>10.85714285714286</v>
+      </c>
+      <c r="R179">
+        <v>416.9479625178905</v>
+      </c>
+      <c r="S179">
+        <v>455.9786563182149</v>
+      </c>
+      <c r="T179">
+        <v>10.51014633357588</v>
+      </c>
+      <c r="U179">
+        <v>12.24199544525758</v>
+      </c>
+    </row>
+    <row r="180" spans="1:21">
+      <c r="A180" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B180">
+        <v>2324</v>
+      </c>
+      <c r="C180">
+        <v>1131</v>
+      </c>
+      <c r="D180">
+        <v>102</v>
+      </c>
+      <c r="E180">
+        <v>2149</v>
+      </c>
+      <c r="F180">
+        <v>73</v>
+      </c>
+      <c r="G180">
+        <v>2</v>
+      </c>
+      <c r="H180">
+        <v>-1.285714285714286</v>
+      </c>
+      <c r="I180">
+        <v>2.816901408450704</v>
+      </c>
+      <c r="J180">
+        <v>-1.037470651975196</v>
+      </c>
+      <c r="K180">
+        <v>8</v>
+      </c>
+      <c r="L180">
+        <v>3</v>
+      </c>
+      <c r="M180">
+        <v>9.571428571428571</v>
+      </c>
+      <c r="N180">
+        <v>0</v>
+      </c>
+      <c r="O180">
+        <v>0</v>
+      </c>
+      <c r="P180">
+        <v>6</v>
+      </c>
+      <c r="Q180">
+        <v>10.85714285714286</v>
+      </c>
+      <c r="R180">
+        <v>418.388197276156</v>
+      </c>
+      <c r="S180">
+        <v>457.1913655105506</v>
+      </c>
+      <c r="T180">
+        <v>10.10590993613065</v>
+      </c>
+      <c r="U180">
+        <v>11.34184872134158</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21">
+      <c r="A181" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B181">
+        <v>2333</v>
+      </c>
+      <c r="C181">
+        <v>1136</v>
+      </c>
+      <c r="D181">
+        <v>102</v>
+      </c>
+      <c r="E181">
+        <v>2156</v>
+      </c>
+      <c r="F181">
+        <v>75</v>
+      </c>
+      <c r="G181">
+        <v>2</v>
+      </c>
+      <c r="H181">
+        <v>-4.428571428571429</v>
+      </c>
+      <c r="I181">
+        <v>2.73972602739726</v>
+      </c>
+      <c r="J181">
+        <v>-4.874558132331404</v>
+      </c>
+      <c r="K181">
+        <v>9</v>
+      </c>
+      <c r="L181">
+        <v>5</v>
+      </c>
+      <c r="M181">
+        <v>6</v>
+      </c>
+      <c r="N181">
+        <v>0</v>
+      </c>
+      <c r="O181">
+        <v>0</v>
+      </c>
+      <c r="P181">
+        <v>7</v>
+      </c>
+      <c r="Q181">
+        <v>10.42857142857143</v>
+      </c>
+      <c r="R181">
+        <v>420.0084613792048</v>
+      </c>
+      <c r="S181">
+        <v>459.2125474977767</v>
+      </c>
+      <c r="T181">
+        <v>9.701673538685423</v>
+      </c>
+      <c r="U181">
+        <v>10.62173134220878</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21">
+      <c r="A182" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B182">
+        <v>2348</v>
+      </c>
+      <c r="C182">
+        <v>1140</v>
+      </c>
+      <c r="D182">
+        <v>102</v>
+      </c>
+      <c r="E182">
+        <v>2163</v>
+      </c>
+      <c r="F182">
+        <v>83</v>
+      </c>
+      <c r="G182">
+        <v>8</v>
+      </c>
+      <c r="H182">
+        <v>-4.428571428571429</v>
+      </c>
+      <c r="I182">
+        <v>10.66666666666667</v>
+      </c>
+      <c r="J182">
+        <v>-4.874558132331404</v>
+      </c>
+      <c r="K182">
+        <v>15</v>
+      </c>
+      <c r="L182">
+        <v>4</v>
+      </c>
+      <c r="M182">
+        <v>6</v>
+      </c>
+      <c r="N182">
+        <v>0</v>
+      </c>
+      <c r="O182">
+        <v>0</v>
+      </c>
+      <c r="P182">
+        <v>7</v>
+      </c>
+      <c r="Q182">
+        <v>10.42857142857143</v>
+      </c>
+      <c r="R182">
+        <v>422.7089015509528</v>
+      </c>
+      <c r="S182">
+        <v>460.8294930875576</v>
+      </c>
+      <c r="T182">
+        <v>10.51014633357588</v>
+      </c>
+      <c r="U182">
+        <v>12.06196610047438</v>
+      </c>
+    </row>
+    <row r="183" spans="1:21">
+      <c r="A183" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B183">
+        <v>2348</v>
+      </c>
+      <c r="C183">
+        <v>1140</v>
+      </c>
+      <c r="D183">
+        <v>102</v>
+      </c>
+      <c r="E183">
+        <v>2163</v>
+      </c>
+      <c r="F183">
+        <v>83</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>-2</v>
+      </c>
+      <c r="I183">
+        <v>0</v>
+      </c>
+      <c r="J183">
+        <v>-2.231617965175817</v>
+      </c>
+      <c r="K183">
+        <v>0</v>
+      </c>
+      <c r="L183">
+        <v>0</v>
+      </c>
+      <c r="M183">
+        <v>6.714285714285714</v>
+      </c>
+      <c r="N183">
+        <v>0</v>
+      </c>
+      <c r="O183">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P183">
+        <v>0</v>
+      </c>
+      <c r="Q183">
+        <v>8.571428571428571</v>
+      </c>
+      <c r="R183">
+        <v>422.7089015509528</v>
+      </c>
+      <c r="S183">
+        <v>460.8294930875576</v>
+      </c>
+      <c r="T183">
+        <v>10.51014633357588</v>
+      </c>
+      <c r="U183">
+        <v>12.06196610047438</v>
+      </c>
+    </row>
+    <row r="184" spans="1:21">
+      <c r="A184" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B184">
+        <v>2353</v>
+      </c>
+      <c r="C184">
+        <v>1144</v>
+      </c>
+      <c r="D184">
+        <v>102</v>
+      </c>
+      <c r="E184">
+        <v>2193</v>
+      </c>
+      <c r="F184">
+        <v>58</v>
+      </c>
+      <c r="G184">
+        <v>-25</v>
+      </c>
+      <c r="H184">
+        <v>-3.142857142857143</v>
+      </c>
+      <c r="I184">
+        <v>-30.12048192771084</v>
+      </c>
+      <c r="J184">
+        <v>-4.137791850593587</v>
+      </c>
+      <c r="K184">
+        <v>5</v>
+      </c>
+      <c r="L184">
+        <v>4</v>
+      </c>
+      <c r="M184">
+        <v>6.571428571428571</v>
+      </c>
+      <c r="N184">
+        <v>0</v>
+      </c>
+      <c r="O184">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P184">
+        <v>30</v>
+      </c>
+      <c r="Q184">
+        <v>9.571428571428571</v>
+      </c>
+      <c r="R184">
+        <v>423.6090482748688</v>
+      </c>
+      <c r="S184">
+        <v>462.4464386773385</v>
+      </c>
+      <c r="T184">
+        <v>7.276255154014067</v>
+      </c>
+      <c r="U184">
+        <v>7.561232480894385</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21">
+      <c r="A185" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B185">
+        <v>2353</v>
+      </c>
+      <c r="C185">
+        <v>1144</v>
+      </c>
+      <c r="D185">
+        <v>102</v>
+      </c>
+      <c r="E185">
+        <v>2193</v>
+      </c>
+      <c r="F185">
+        <v>58</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>-3.428571428571428</v>
+      </c>
+      <c r="I185">
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>-4.52918128307891</v>
+      </c>
+      <c r="K185">
+        <v>0</v>
+      </c>
+      <c r="L185">
+        <v>0</v>
+      </c>
+      <c r="M185">
+        <v>6.428571428571429</v>
+      </c>
+      <c r="N185">
+        <v>0</v>
+      </c>
+      <c r="O185">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P185">
+        <v>0</v>
+      </c>
+      <c r="Q185">
+        <v>9.714285714285714</v>
+      </c>
+      <c r="R185">
+        <v>423.6090482748688</v>
+      </c>
+      <c r="S185">
+        <v>462.4464386773385</v>
+      </c>
+      <c r="T185">
+        <v>7.276255154014067</v>
+      </c>
+      <c r="U185">
+        <v>7.561232480894385</v>
+      </c>
+    </row>
+    <row r="186" spans="1:21">
+      <c r="A186" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B186">
+        <v>2363</v>
+      </c>
+      <c r="C186">
+        <v>1149</v>
+      </c>
+      <c r="D186">
+        <v>103</v>
+      </c>
+      <c r="E186">
+        <v>2203</v>
+      </c>
+      <c r="F186">
+        <v>57</v>
+      </c>
+      <c r="G186">
+        <v>-1</v>
+      </c>
+      <c r="H186">
+        <v>-5.285714285714286</v>
+      </c>
+      <c r="I186">
+        <v>-1.724137931034483</v>
+      </c>
+      <c r="J186">
+        <v>-7.45355103097807</v>
+      </c>
+      <c r="K186">
+        <v>10</v>
+      </c>
+      <c r="L186">
+        <v>5</v>
+      </c>
+      <c r="M186">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="N186">
+        <v>1</v>
+      </c>
+      <c r="O186">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P186">
+        <v>10</v>
+      </c>
+      <c r="Q186">
+        <v>10.28571428571429</v>
+      </c>
+      <c r="R186">
+        <v>425.4093417227008</v>
+      </c>
+      <c r="S186">
+        <v>464.4676206645646</v>
+      </c>
+      <c r="T186">
+        <v>8.488964346349746</v>
+      </c>
+      <c r="U186">
+        <v>8.461379204810385</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21">
+      <c r="A187" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B187">
+        <v>2370</v>
+      </c>
+      <c r="C187">
+        <v>1151</v>
+      </c>
+      <c r="D187">
+        <v>103</v>
+      </c>
+      <c r="E187">
+        <v>2216</v>
+      </c>
+      <c r="F187">
+        <v>51</v>
+      </c>
+      <c r="G187">
+        <v>-6</v>
+      </c>
+      <c r="H187">
+        <v>-5.285714285714286</v>
+      </c>
+      <c r="I187">
+        <v>-10.52631578947368</v>
+      </c>
+      <c r="J187">
+        <v>-7.45355103097807</v>
+      </c>
+      <c r="K187">
+        <v>7</v>
+      </c>
+      <c r="L187">
+        <v>2</v>
+      </c>
+      <c r="M187">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="N187">
+        <v>0</v>
+      </c>
+      <c r="O187">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P187">
+        <v>13</v>
+      </c>
+      <c r="Q187">
+        <v>10.28571428571429</v>
+      </c>
+      <c r="R187">
+        <v>426.6695471361832</v>
+      </c>
+      <c r="S187">
+        <v>465.2760934594551</v>
+      </c>
+      <c r="T187">
+        <v>8.08472794890452</v>
+      </c>
+      <c r="U187">
+        <v>8.281349860027184</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21">
+      <c r="A188" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B188">
+        <v>2378</v>
+      </c>
+      <c r="C188">
+        <v>1157</v>
+      </c>
+      <c r="D188">
+        <v>103</v>
+      </c>
+      <c r="E188">
+        <v>2224</v>
+      </c>
+      <c r="F188">
+        <v>51</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>-2.714285714285714</v>
+      </c>
+      <c r="I188">
+        <v>0</v>
+      </c>
+      <c r="J188">
+        <v>-5.324538084783354</v>
+      </c>
+      <c r="K188">
+        <v>8</v>
+      </c>
+      <c r="L188">
+        <v>6</v>
+      </c>
+      <c r="M188">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="N188">
+        <v>0</v>
+      </c>
+      <c r="O188">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P188">
+        <v>8</v>
+      </c>
+      <c r="Q188">
+        <v>7.714285714285714</v>
+      </c>
+      <c r="R188">
+        <v>428.1097818944488</v>
+      </c>
+      <c r="S188">
+        <v>467.7015118441264</v>
+      </c>
+      <c r="T188">
+        <v>8.488964346349746</v>
+      </c>
+      <c r="U188">
+        <v>8.101320515243984</v>
+      </c>
+    </row>
+    <row r="189" spans="1:21">
+      <c r="A189" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B189">
+        <v>2384</v>
+      </c>
+      <c r="C189">
+        <v>1161</v>
+      </c>
+      <c r="D189">
+        <v>103</v>
+      </c>
+      <c r="E189">
+        <v>2235</v>
+      </c>
+      <c r="F189">
+        <v>46</v>
+      </c>
+      <c r="G189">
+        <v>-5</v>
+      </c>
+      <c r="H189">
+        <v>-2.714285714285714</v>
+      </c>
+      <c r="I189">
+        <v>-9.803921568627452</v>
+      </c>
+      <c r="J189">
+        <v>-5.324538084783354</v>
+      </c>
+      <c r="K189">
+        <v>6</v>
+      </c>
+      <c r="L189">
+        <v>4</v>
+      </c>
+      <c r="M189">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="N189">
+        <v>0</v>
+      </c>
+      <c r="O189">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P189">
+        <v>11</v>
+      </c>
+      <c r="Q189">
+        <v>7.714285714285714</v>
+      </c>
+      <c r="R189">
+        <v>429.189957963148</v>
+      </c>
+      <c r="S189">
+        <v>469.3184574339073</v>
+      </c>
+      <c r="T189">
+        <v>8.488964346349746</v>
+      </c>
+      <c r="U189">
+        <v>6.481056412195188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21">
+      <c r="A190" s="2">
+        <v>44079</v>
+      </c>
+      <c r="B190">
+        <v>2384</v>
+      </c>
+      <c r="C190">
+        <v>1161</v>
+      </c>
+      <c r="D190">
+        <v>103</v>
+      </c>
+      <c r="E190">
+        <v>2235</v>
+      </c>
+      <c r="F190">
+        <v>46</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
+      <c r="H190">
+        <v>-3.571428571428572</v>
+      </c>
+      <c r="I190">
+        <v>0</v>
+      </c>
+      <c r="J190">
+        <v>-7.642335230166706</v>
+      </c>
+      <c r="K190">
+        <v>0</v>
+      </c>
+      <c r="L190">
+        <v>0</v>
+      </c>
+      <c r="M190">
+        <v>4.285714285714286</v>
+      </c>
+      <c r="N190">
+        <v>0</v>
+      </c>
+      <c r="O190">
+        <v>0</v>
+      </c>
+      <c r="P190">
+        <v>0</v>
+      </c>
+      <c r="Q190">
+        <v>7.857142857142857</v>
+      </c>
+      <c r="R190">
+        <v>429.189957963148</v>
+      </c>
+      <c r="S190">
+        <v>469.3184574339073</v>
+      </c>
+      <c r="T190">
+        <v>8.488964346349746</v>
+      </c>
+      <c r="U190">
+        <v>6.481056412195188</v>
+      </c>
+    </row>
+    <row r="191" spans="1:21">
+      <c r="A191" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B191">
+        <v>2389</v>
+      </c>
+      <c r="C191">
+        <v>1164</v>
+      </c>
+      <c r="D191">
+        <v>103</v>
+      </c>
+      <c r="E191">
+        <v>2247</v>
+      </c>
+      <c r="F191">
+        <v>39</v>
+      </c>
+      <c r="G191">
+        <v>-7</v>
+      </c>
+      <c r="H191">
+        <v>-2</v>
+      </c>
+      <c r="I191">
+        <v>-15.21739130434783</v>
+      </c>
+      <c r="J191">
+        <v>-3.906432974527608</v>
+      </c>
+      <c r="K191">
+        <v>5</v>
+      </c>
+      <c r="L191">
+        <v>3</v>
+      </c>
+      <c r="M191">
+        <v>4.285714285714286</v>
+      </c>
+      <c r="N191">
+        <v>0</v>
+      </c>
+      <c r="O191">
+        <v>0</v>
+      </c>
+      <c r="P191">
+        <v>12</v>
+      </c>
+      <c r="Q191">
+        <v>6.285714285714286</v>
+      </c>
+      <c r="R191">
+        <v>430.090104687064</v>
+      </c>
+      <c r="S191">
+        <v>470.531166626243</v>
+      </c>
+      <c r="T191">
+        <v>8.08472794890452</v>
+      </c>
+      <c r="U191">
+        <v>6.481056412195188</v>
+      </c>
+    </row>
+    <row r="192" spans="1:21">
+      <c r="A192" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B192">
+        <v>2389</v>
+      </c>
+      <c r="C192">
+        <v>1164</v>
+      </c>
+      <c r="D192">
+        <v>103</v>
+      </c>
+      <c r="E192">
+        <v>2247</v>
+      </c>
+      <c r="F192">
+        <v>39</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>-0.7142857142857143</v>
+      </c>
+      <c r="I192">
+        <v>0</v>
+      </c>
+      <c r="J192">
+        <v>-0.431529499624133</v>
+      </c>
+      <c r="K192">
+        <v>0</v>
+      </c>
+      <c r="L192">
+        <v>0</v>
+      </c>
+      <c r="M192">
+        <v>4.857142857142857</v>
+      </c>
+      <c r="N192">
+        <v>0</v>
+      </c>
+      <c r="O192">
+        <v>0</v>
+      </c>
+      <c r="P192">
+        <v>0</v>
+      </c>
+      <c r="Q192">
+        <v>5.571428571428571</v>
+      </c>
+      <c r="R192">
+        <v>430.090104687064</v>
+      </c>
+      <c r="S192">
+        <v>470.531166626243</v>
+      </c>
+      <c r="T192">
+        <v>8.08472794890452</v>
+      </c>
+      <c r="U192">
+        <v>6.481056412195188</v>
+      </c>
+    </row>
+    <row r="193" spans="1:21">
+      <c r="A193" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B193">
+        <v>2393</v>
+      </c>
+      <c r="C193">
+        <v>1166</v>
+      </c>
+      <c r="D193">
+        <v>103</v>
+      </c>
+      <c r="E193">
+        <v>2258</v>
+      </c>
+      <c r="F193">
+        <v>32</v>
+      </c>
+      <c r="G193">
+        <v>-7</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193">
+        <v>-17.94871794871795</v>
+      </c>
+      <c r="J193">
+        <v>0.969030724465503</v>
+      </c>
+      <c r="K193">
+        <v>4</v>
+      </c>
+      <c r="L193">
+        <v>2</v>
+      </c>
+      <c r="M193">
+        <v>4</v>
+      </c>
+      <c r="N193">
+        <v>0</v>
+      </c>
+      <c r="O193">
+        <v>0</v>
+      </c>
+      <c r="P193">
+        <v>11</v>
+      </c>
+      <c r="Q193">
+        <v>4</v>
+      </c>
+      <c r="R193">
+        <v>430.8102220661968</v>
+      </c>
+      <c r="S193">
+        <v>471.3396394211334</v>
+      </c>
+      <c r="T193">
+        <v>6.872018756568841</v>
+      </c>
+      <c r="U193">
+        <v>5.40088034349599</v>
+      </c>
+    </row>
+    <row r="194" spans="1:21">
+      <c r="A194" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B194">
+        <v>2400</v>
+      </c>
+      <c r="C194">
+        <v>1171</v>
+      </c>
+      <c r="D194">
+        <v>103</v>
+      </c>
+      <c r="E194">
+        <v>2260</v>
+      </c>
+      <c r="F194">
+        <v>37</v>
+      </c>
+      <c r="G194">
+        <v>5</v>
+      </c>
+      <c r="H194">
+        <v>1.285714285714286</v>
+      </c>
+      <c r="I194">
+        <v>15.625</v>
+      </c>
+      <c r="J194">
+        <v>3.764061780366124</v>
+      </c>
+      <c r="K194">
+        <v>7</v>
+      </c>
+      <c r="L194">
+        <v>5</v>
+      </c>
+      <c r="M194">
+        <v>6.428571428571429</v>
+      </c>
+      <c r="N194">
+        <v>0</v>
+      </c>
+      <c r="O194">
+        <v>0</v>
+      </c>
+      <c r="P194">
+        <v>2</v>
+      </c>
+      <c r="Q194">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="R194">
+        <v>432.0704274796792</v>
+      </c>
+      <c r="S194">
+        <v>473.3608214083596</v>
+      </c>
+      <c r="T194">
+        <v>8.08472794890452</v>
+      </c>
+      <c r="U194">
+        <v>5.40088034349599</v>
+      </c>
+    </row>
+    <row r="195" spans="1:21">
+      <c r="A195" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B195">
+        <v>2412</v>
+      </c>
+      <c r="C195">
+        <v>1178</v>
+      </c>
+      <c r="D195">
+        <v>103</v>
+      </c>
+      <c r="E195">
+        <v>2263</v>
+      </c>
+      <c r="F195">
+        <v>46</v>
+      </c>
+      <c r="G195">
+        <v>9</v>
+      </c>
+      <c r="H195">
+        <v>2.285714285714286</v>
+      </c>
+      <c r="I195">
+        <v>24.32432432432433</v>
+      </c>
+      <c r="J195">
+        <v>5.937974823844385</v>
+      </c>
+      <c r="K195">
+        <v>12</v>
+      </c>
+      <c r="L195">
+        <v>7</v>
+      </c>
+      <c r="M195">
+        <v>5.714285714285714</v>
+      </c>
+      <c r="N195">
+        <v>0</v>
+      </c>
+      <c r="O195">
+        <v>0</v>
+      </c>
+      <c r="P195">
+        <v>3</v>
+      </c>
+      <c r="Q195">
+        <v>3.428571428571428</v>
+      </c>
+      <c r="R195">
+        <v>434.2307796170776</v>
+      </c>
+      <c r="S195">
+        <v>476.1904761904763</v>
+      </c>
+      <c r="T195">
+        <v>8.488964346349746</v>
+      </c>
+      <c r="U195">
+        <v>6.120997722628789</v>
+      </c>
+    </row>
+    <row r="196" spans="1:21">
+      <c r="A196" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B196">
+        <v>2412</v>
+      </c>
+      <c r="C196">
+        <v>1178</v>
+      </c>
+      <c r="D196">
+        <v>103</v>
+      </c>
+      <c r="E196">
+        <v>2263</v>
+      </c>
+      <c r="F196">
+        <v>46</v>
+      </c>
+      <c r="G196">
+        <v>0</v>
+      </c>
+      <c r="H196">
+        <v>2.285714285714286</v>
+      </c>
+      <c r="I196">
+        <v>0</v>
+      </c>
+      <c r="J196">
+        <v>5.937974823844385</v>
+      </c>
+      <c r="K196">
+        <v>0</v>
+      </c>
+      <c r="L196">
+        <v>0</v>
+      </c>
+      <c r="M196">
+        <v>5.714285714285714</v>
+      </c>
+      <c r="N196">
+        <v>0</v>
+      </c>
+      <c r="O196">
+        <v>0</v>
+      </c>
+      <c r="P196">
+        <v>0</v>
+      </c>
+      <c r="Q196">
+        <v>3.428571428571428</v>
+      </c>
+      <c r="R196">
+        <v>434.2307796170776</v>
+      </c>
+      <c r="S196">
+        <v>476.1904761904763</v>
+      </c>
+      <c r="T196">
+        <v>6.872018756568841</v>
+      </c>
+      <c r="U196">
+        <v>5.040821653929591</v>
+      </c>
+    </row>
+    <row r="197" spans="1:21">
+      <c r="A197" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B197">
+        <v>2429</v>
+      </c>
+      <c r="C197">
+        <v>1186</v>
+      </c>
+      <c r="D197">
+        <v>103</v>
+      </c>
+      <c r="E197">
+        <v>2271</v>
+      </c>
+      <c r="F197">
+        <v>55</v>
+      </c>
+      <c r="G197">
+        <v>9</v>
+      </c>
+      <c r="H197">
+        <v>7.714285714285714</v>
+      </c>
+      <c r="I197">
+        <v>19.56521739130435</v>
+      </c>
+      <c r="J197">
+        <v>16.554025439895</v>
+      </c>
+      <c r="K197">
+        <v>17</v>
+      </c>
+      <c r="L197">
+        <v>8</v>
+      </c>
+      <c r="M197">
+        <v>12</v>
+      </c>
+      <c r="N197">
+        <v>0</v>
+      </c>
+      <c r="O197">
+        <v>0</v>
+      </c>
+      <c r="P197">
+        <v>8</v>
+      </c>
+      <c r="Q197">
+        <v>4.285714285714286</v>
+      </c>
+      <c r="R197">
+        <v>437.291278478392</v>
+      </c>
+      <c r="S197">
+        <v>479.4243673700381</v>
+      </c>
+      <c r="T197">
+        <v>10.10590993613065</v>
+      </c>
+      <c r="U197">
+        <v>8.101320515243984</v>
+      </c>
+    </row>
+    <row r="198" spans="1:21">
+      <c r="A198" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B198">
+        <v>2429</v>
+      </c>
+      <c r="C198">
+        <v>1186</v>
+      </c>
+      <c r="D198">
+        <v>103</v>
+      </c>
+      <c r="E198">
+        <v>2271</v>
+      </c>
+      <c r="F198">
+        <v>55</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>9.428571428571429</v>
+      </c>
+      <c r="I198">
+        <v>0</v>
+      </c>
+      <c r="J198">
+        <v>17.14580284853287</v>
+      </c>
+      <c r="K198">
+        <v>0</v>
+      </c>
+      <c r="L198">
+        <v>0</v>
+      </c>
+      <c r="M198">
+        <v>14.71428571428571</v>
+      </c>
+      <c r="N198">
+        <v>0</v>
+      </c>
+      <c r="O198">
+        <v>0</v>
+      </c>
+      <c r="P198">
+        <v>0</v>
+      </c>
+      <c r="Q198">
+        <v>5.285714285714286</v>
+      </c>
+      <c r="R198">
+        <v>437.291278478392</v>
+      </c>
+      <c r="S198">
+        <v>479.4243673700381</v>
+      </c>
+      <c r="T198">
+        <v>8.893200743794972</v>
+      </c>
+      <c r="U198">
+        <v>7.201173791327986</v>
+      </c>
+    </row>
+    <row r="199" spans="1:21">
+      <c r="A199" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B199">
+        <v>2429</v>
+      </c>
+      <c r="C199">
+        <v>1186</v>
+      </c>
+      <c r="D199">
+        <v>103</v>
+      </c>
+      <c r="E199">
+        <v>2271</v>
+      </c>
+      <c r="F199">
+        <v>55</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>9.142857142857142</v>
+      </c>
+      <c r="I199">
+        <v>0</v>
+      </c>
+      <c r="J199">
+        <v>14.64177316003717</v>
+      </c>
+      <c r="K199">
+        <v>0</v>
+      </c>
+      <c r="L199">
+        <v>0</v>
+      </c>
+      <c r="M199">
+        <v>15.71428571428571</v>
+      </c>
+      <c r="N199">
+        <v>0</v>
+      </c>
+      <c r="O199">
+        <v>0</v>
+      </c>
+      <c r="P199">
+        <v>0</v>
+      </c>
+      <c r="Q199">
+        <v>6.571428571428571</v>
+      </c>
+      <c r="R199">
+        <v>437.291278478392</v>
+      </c>
+      <c r="S199">
+        <v>479.4243673700381</v>
+      </c>
+      <c r="T199">
+        <v>8.893200743794972</v>
+      </c>
+      <c r="U199">
+        <v>7.201173791327986</v>
+      </c>
+    </row>
+    <row r="200" spans="1:21">
+      <c r="A200" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B200">
+        <v>2477</v>
+      </c>
+      <c r="C200">
+        <v>1210</v>
+      </c>
+      <c r="D200">
+        <v>103</v>
+      </c>
+      <c r="E200">
+        <v>2288</v>
+      </c>
+      <c r="F200">
+        <v>86</v>
+      </c>
+      <c r="G200">
+        <v>31</v>
+      </c>
+      <c r="H200">
+        <v>10.71428571428571</v>
+      </c>
+      <c r="I200">
+        <v>56.36363636363636</v>
+      </c>
+      <c r="J200">
+        <v>16.0703445886086</v>
+      </c>
+      <c r="K200">
+        <v>48</v>
+      </c>
+      <c r="L200">
+        <v>24</v>
+      </c>
+      <c r="M200">
+        <v>19.71428571428572</v>
+      </c>
+      <c r="N200">
+        <v>0</v>
+      </c>
+      <c r="O200">
+        <v>0</v>
+      </c>
+      <c r="P200">
+        <v>17</v>
+      </c>
+      <c r="Q200">
+        <v>9</v>
+      </c>
+      <c r="R200">
+        <v>445.9326870279855</v>
+      </c>
+      <c r="S200">
+        <v>489.1260409087234</v>
+      </c>
+      <c r="T200">
+        <v>17.78640148758994</v>
+      </c>
+      <c r="U200">
+        <v>15.12246496178877</v>
+      </c>
+    </row>
+    <row r="201" spans="1:21">
+      <c r="A201" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B201">
+        <v>2503</v>
+      </c>
+      <c r="C201">
+        <v>1224</v>
+      </c>
+      <c r="D201">
+        <v>103</v>
+      </c>
+      <c r="E201">
+        <v>2297</v>
+      </c>
+      <c r="F201">
+        <v>103</v>
+      </c>
+      <c r="G201">
+        <v>17</v>
+      </c>
+      <c r="H201">
+        <v>9.428571428571429</v>
+      </c>
+      <c r="I201">
+        <v>19.76744186046512</v>
+      </c>
+      <c r="J201">
+        <v>13.27531353270797</v>
+      </c>
+      <c r="K201">
+        <v>26</v>
+      </c>
+      <c r="L201">
+        <v>14</v>
+      </c>
+      <c r="M201">
+        <v>17.28571428571428</v>
+      </c>
+      <c r="N201">
+        <v>0</v>
+      </c>
+      <c r="O201">
+        <v>0</v>
+      </c>
+      <c r="P201">
+        <v>9</v>
+      </c>
+      <c r="Q201">
+        <v>7.857142857142857</v>
+      </c>
+      <c r="R201">
+        <v>450.6134499923487</v>
+      </c>
+      <c r="S201">
+        <v>494.7853504729566</v>
+      </c>
+      <c r="T201">
+        <v>21.42452906459697</v>
+      </c>
+      <c r="U201">
+        <v>18.54302251266957</v>
+      </c>
+    </row>
+    <row r="202" spans="1:21">
+      <c r="A202" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B202">
+        <v>2522</v>
+      </c>
+      <c r="C202">
+        <v>1232</v>
+      </c>
+      <c r="D202">
+        <v>103</v>
+      </c>
+      <c r="E202">
+        <v>2309</v>
+      </c>
+      <c r="F202">
+        <v>110</v>
+      </c>
+      <c r="G202">
+        <v>7</v>
+      </c>
+      <c r="H202">
+        <v>8.428571428571429</v>
+      </c>
+      <c r="I202">
+        <v>6.796116504854369</v>
+      </c>
+      <c r="J202">
+        <v>12.44886725171624</v>
+      </c>
+      <c r="K202">
+        <v>19</v>
+      </c>
+      <c r="L202">
+        <v>8</v>
+      </c>
+      <c r="M202">
+        <v>19.85714285714286</v>
+      </c>
+      <c r="N202">
+        <v>0</v>
+      </c>
+      <c r="O202">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P202">
+        <v>12</v>
+      </c>
+      <c r="Q202">
+        <v>11.28571428571429</v>
+      </c>
+      <c r="R202">
+        <v>454.0340075432295</v>
+      </c>
+      <c r="S202">
+        <v>498.0192416525184</v>
+      </c>
+      <c r="T202">
+        <v>21.8287654620422</v>
+      </c>
+      <c r="U202">
+        <v>19.80322792615196</v>
+      </c>
+    </row>
+    <row r="203" spans="1:21">
+      <c r="A203" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B203">
+        <v>2550</v>
+      </c>
+      <c r="C203">
+        <v>1248</v>
+      </c>
+      <c r="D203">
+        <v>103</v>
+      </c>
+      <c r="E203">
+        <v>2326</v>
+      </c>
+      <c r="F203">
+        <v>121</v>
+      </c>
+      <c r="G203">
+        <v>11</v>
+      </c>
+      <c r="H203">
+        <v>8.428571428571429</v>
+      </c>
+      <c r="I203">
+        <v>10</v>
+      </c>
+      <c r="J203">
+        <v>12.44886725171624</v>
+      </c>
+      <c r="K203">
+        <v>28</v>
+      </c>
+      <c r="L203">
+        <v>16</v>
+      </c>
+      <c r="M203">
+        <v>19.85714285714286</v>
+      </c>
+      <c r="N203">
+        <v>0</v>
+      </c>
+      <c r="O203">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P203">
+        <v>17</v>
+      </c>
+      <c r="Q203">
+        <v>11.28571428571429</v>
+      </c>
+      <c r="R203">
+        <v>459.0748291971591</v>
+      </c>
+      <c r="S203">
+        <v>504.4870240116419</v>
+      </c>
+      <c r="T203">
+        <v>28.29654782116582</v>
+      </c>
+      <c r="U203">
+        <v>24.84404958008156</v>
+      </c>
+    </row>
+    <row r="204" spans="1:21">
+      <c r="A204" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B204">
+        <v>2550</v>
+      </c>
+      <c r="C204">
+        <v>1248</v>
+      </c>
+      <c r="D204">
+        <v>103</v>
+      </c>
+      <c r="E204">
+        <v>2326</v>
+      </c>
+      <c r="F204">
+        <v>121</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>3.571428571428572</v>
+      </c>
+      <c r="I204">
+        <v>0</v>
+      </c>
+      <c r="J204">
+        <v>4.020979350144127</v>
+      </c>
+      <c r="K204">
+        <v>0</v>
+      </c>
+      <c r="L204">
+        <v>0</v>
+      </c>
+      <c r="M204">
+        <v>15.28571428571429</v>
+      </c>
+      <c r="N204">
+        <v>0</v>
+      </c>
+      <c r="O204">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P204">
+        <v>0</v>
+      </c>
+      <c r="Q204">
+        <v>11.57142857142857</v>
+      </c>
+      <c r="R204">
+        <v>459.0748291971591</v>
+      </c>
+      <c r="S204">
+        <v>504.4870240116419</v>
+      </c>
+      <c r="T204">
+        <v>25.06265664160401</v>
+      </c>
+      <c r="U204">
+        <v>21.78355071876716</v>
+      </c>
+    </row>
+    <row r="205" spans="1:21">
+      <c r="A205" s="2">
+        <v>44094</v>
+      </c>
+      <c r="B205">
+        <v>2568</v>
+      </c>
+      <c r="C205">
+        <v>1252</v>
+      </c>
+      <c r="D205">
+        <v>104</v>
+      </c>
+      <c r="E205">
+        <v>2350</v>
+      </c>
+      <c r="F205">
+        <v>114</v>
+      </c>
+      <c r="G205">
+        <v>-7</v>
+      </c>
+      <c r="H205">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I205">
+        <v>-5.785123966942149</v>
+      </c>
+      <c r="J205">
+        <v>0.9396588269631388</v>
+      </c>
+      <c r="K205">
+        <v>18</v>
+      </c>
+      <c r="L205">
+        <v>4</v>
+      </c>
+      <c r="M205">
+        <v>13.85714285714286</v>
+      </c>
+      <c r="N205">
+        <v>1</v>
+      </c>
+      <c r="O205">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P205">
+        <v>24</v>
+      </c>
+      <c r="Q205">
+        <v>12.85714285714286</v>
+      </c>
+      <c r="R205">
+        <v>462.3153574032568</v>
+      </c>
+      <c r="S205">
+        <v>506.1039696014229</v>
+      </c>
+      <c r="T205">
+        <v>26.67960223138492</v>
+      </c>
+      <c r="U205">
+        <v>25.02407892486475</v>
+      </c>
+    </row>
+    <row r="206" spans="1:21">
+      <c r="A206" s="2">
+        <v>44095</v>
+      </c>
+      <c r="B206">
+        <v>2568</v>
+      </c>
+      <c r="C206">
+        <v>1252</v>
+      </c>
+      <c r="D206">
+        <v>104</v>
+      </c>
+      <c r="E206">
+        <v>2350</v>
+      </c>
+      <c r="F206">
+        <v>114</v>
+      </c>
+      <c r="G206">
+        <v>0</v>
+      </c>
+      <c r="H206">
+        <v>1.285714285714286</v>
+      </c>
+      <c r="I206">
+        <v>0</v>
+      </c>
+      <c r="J206">
+        <v>1.279401030070444</v>
+      </c>
+      <c r="K206">
+        <v>0</v>
+      </c>
+      <c r="L206">
+        <v>0</v>
+      </c>
+      <c r="M206">
+        <v>14.14285714285714</v>
+      </c>
+      <c r="N206">
+        <v>0</v>
+      </c>
+      <c r="O206">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P206">
+        <v>0</v>
+      </c>
+      <c r="Q206">
+        <v>12.71428571428571</v>
+      </c>
+      <c r="R206">
+        <v>462.3153574032568</v>
+      </c>
+      <c r="S206">
+        <v>506.1039696014229</v>
+      </c>
+      <c r="T206">
+        <v>26.67960223138492</v>
+      </c>
+      <c r="U206">
+        <v>25.02407892486475</v>
+      </c>
+    </row>
+    <row r="207" spans="1:21">
+      <c r="A207" s="2">
+        <v>44096</v>
+      </c>
+      <c r="B207">
+        <v>2584</v>
+      </c>
+      <c r="C207">
+        <v>1261</v>
+      </c>
+      <c r="D207">
+        <v>104</v>
+      </c>
+      <c r="E207">
+        <v>2369</v>
+      </c>
+      <c r="F207">
+        <v>111</v>
+      </c>
+      <c r="G207">
+        <v>-3</v>
+      </c>
+      <c r="H207">
+        <v>0.4285714285714285</v>
+      </c>
+      <c r="I207">
+        <v>-2.631578947368421</v>
+      </c>
+      <c r="J207">
+        <v>0.4510696975374309</v>
+      </c>
+      <c r="K207">
+        <v>16</v>
+      </c>
+      <c r="L207">
+        <v>9</v>
+      </c>
+      <c r="M207">
+        <v>13.28571428571429</v>
+      </c>
+      <c r="N207">
+        <v>0</v>
+      </c>
+      <c r="O207">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="P207">
+        <v>19</v>
+      </c>
+      <c r="Q207">
+        <v>12.71428571428571</v>
+      </c>
+      <c r="R207">
+        <v>465.195826919788</v>
+      </c>
+      <c r="S207">
+        <v>509.74209717843</v>
+      </c>
+      <c r="T207">
+        <v>20.61605626970652</v>
+      </c>
+      <c r="U207">
+        <v>19.26313989180236</v>
+      </c>
+    </row>
+    <row r="208" spans="1:21">
+      <c r="A208" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B208">
+        <v>2600</v>
+      </c>
+      <c r="C208">
+        <v>1268</v>
+      </c>
+      <c r="D208">
+        <v>104</v>
+      </c>
+      <c r="E208">
+        <v>2387</v>
+      </c>
+      <c r="F208">
+        <v>109</v>
+      </c>
+      <c r="G208">
+        <v>-2</v>
+      </c>
+      <c r="I208">
+        <v>-1.801801801801802</v>
+      </c>
+      <c r="K208">
+        <v>16</v>
+      </c>
+      <c r="L208">
+        <v>7</v>
+      </c>
+      <c r="N208">
+        <v>0</v>
+      </c>
+      <c r="P208">
+        <v>18</v>
+      </c>
+      <c r="R208">
+        <v>468.0762964363191</v>
+      </c>
+      <c r="S208">
+        <v>512.5717519605465</v>
+      </c>
+      <c r="T208">
+        <v>17.78640148758994</v>
+      </c>
+      <c r="U208">
+        <v>17.46284644397037</v>
+      </c>
+    </row>
+    <row r="209" spans="1:21">
+      <c r="A209" s="2">
+        <v>44098</v>
+      </c>
+      <c r="B209">
+        <v>2621</v>
+      </c>
+      <c r="C209">
+        <v>1279</v>
+      </c>
+      <c r="D209">
+        <v>104</v>
+      </c>
+      <c r="E209">
+        <v>2398</v>
+      </c>
+      <c r="F209">
+        <v>119</v>
+      </c>
+      <c r="G209">
+        <v>10</v>
+      </c>
+      <c r="I209">
+        <v>9.174311926605505</v>
+      </c>
+      <c r="K209">
+        <v>21</v>
+      </c>
+      <c r="L209">
+        <v>11</v>
+      </c>
+      <c r="N209">
+        <v>0</v>
+      </c>
+      <c r="P209">
+        <v>11</v>
+      </c>
+      <c r="R209">
+        <v>471.8569126767663</v>
+      </c>
+      <c r="S209">
+        <v>517.018352332444</v>
+      </c>
+      <c r="T209">
+        <v>18.99911067992562</v>
+      </c>
+      <c r="U209">
+        <v>17.82290513353677</v>
+      </c>
+    </row>
+    <row r="210" spans="1:21">
+      <c r="A210" s="2">
+        <v>44099</v>
+      </c>
+      <c r="B210">
+        <v>2643</v>
+      </c>
+      <c r="C210">
+        <v>1293</v>
+      </c>
+      <c r="D210">
+        <v>104</v>
+      </c>
+      <c r="E210">
+        <v>2415</v>
+      </c>
+      <c r="F210">
+        <v>124</v>
+      </c>
+      <c r="G210">
+        <v>5</v>
+      </c>
+      <c r="I210">
+        <v>4.201680672268908</v>
+      </c>
+      <c r="K210">
+        <v>22</v>
+      </c>
+      <c r="L210">
+        <v>14</v>
+      </c>
+      <c r="N210">
+        <v>0</v>
+      </c>
+      <c r="P210">
+        <v>17</v>
+      </c>
+      <c r="R210">
+        <v>475.8175582619967</v>
+      </c>
+      <c r="S210">
+        <v>522.6776618966771</v>
+      </c>
+      <c r="T210">
+        <v>18.19063788503517</v>
+      </c>
+      <c r="U210">
+        <v>16.74272906483757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>